<commit_message>
DELFOR complete / Start DELJIT
</commit_message>
<xml_diff>
--- a/res/templates/edi.xlsx
+++ b/res/templates/edi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\edi\res\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\EDI\res\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B26AD5-18D2-4433-AAF3-BD5C193EE50A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31F2C78-2B36-42F0-AC92-F39D69D2B0E0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="0" xr2:uid="{767EFC35-BF66-471E-A260-990474AF76E1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="0" xr2:uid="{767EFC35-BF66-471E-A260-990474AF76E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -159,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -170,20 +170,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -593,143 +596,151 @@
       <c r="P4" s="8"/>
     </row>
     <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
     </row>
     <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
     </row>
     <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
       <c r="O9" s="1"/>
     </row>
     <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
-      <c r="I10" s="6" t="s">
+      <c r="I10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
     </row>
     <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H14" s="7" t="s">
+      <c r="H14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
     </row>
     <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
       <c r="E16" s="3"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
     </row>
     <row r="19" spans="2:16" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5" t="s">
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5" t="s">
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5" t="s">
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5" t="s">
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="H14:J14"/>
+  <mergeCells count="26">
     <mergeCell ref="A4:P4"/>
     <mergeCell ref="B5:O5"/>
     <mergeCell ref="B11:D11"/>
@@ -745,13 +756,17 @@
     <mergeCell ref="I10:K10"/>
     <mergeCell ref="I9:K9"/>
     <mergeCell ref="I8:K8"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="L10:N10"/>
     <mergeCell ref="N19:P19"/>
     <mergeCell ref="K19:M19"/>
     <mergeCell ref="H19:J19"/>
     <mergeCell ref="E19:G19"/>
     <mergeCell ref="B19:D19"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="H14:J14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>

</xml_diff>